<commit_message>
updated prop bet tracker
</commit_message>
<xml_diff>
--- a/scratch/Prop Bets.xlsx
+++ b/scratch/Prop Bets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kjzk13/Desktop/Fun/Betting/Models/Git/NBA/data_repos/gambling_stuff/scratch/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC7D83F4-9138-DA4A-8768-8604B53ED0CC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93BB922B-8629-044D-97BC-C3273E68840E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16220" xr2:uid="{A921039E-F491-3040-A02B-E90974210F5A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9958" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10549" uniqueCount="276">
   <si>
     <t>Date</t>
   </si>
@@ -847,6 +847,24 @@
   <si>
     <t>Cole Anthony</t>
   </si>
+  <si>
+    <t>Kyle Anderson</t>
+  </si>
+  <si>
+    <t>Mychal Mulder</t>
+  </si>
+  <si>
+    <t>Armoni Brooks</t>
+  </si>
+  <si>
+    <t>Milwaukee Brewers</t>
+  </si>
+  <si>
+    <t>Ivica Zubac</t>
+  </si>
+  <si>
+    <t>Furkan Korkmaz</t>
+  </si>
 </sst>
 </file>
 
@@ -906,7 +924,12 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="46">
+  <dxfs count="47">
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color theme="0" tint="-0.499984740745262"/>
@@ -1447,10 +1470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C79C926B-E4E0-6445-8BE2-2104EE8EA8CE}">
-  <dimension ref="A1:N1078"/>
+  <dimension ref="A1:N1142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1053" workbookViewId="0">
-      <selection activeCell="N1079" sqref="N1079"/>
+    <sheetView tabSelected="1" topLeftCell="A1112" workbookViewId="0">
+      <selection activeCell="N1143" sqref="N1143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -45090,235 +45113,2830 @@
         <v>1</v>
       </c>
     </row>
+    <row r="1079" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1079" s="3">
+        <v>44309</v>
+      </c>
+      <c r="B1079" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1079" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1079" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1079" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1079" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1079" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1079" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1079" s="2"/>
+      <c r="J1079" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1079" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1079" s="2">
+        <v>116</v>
+      </c>
+      <c r="M1079" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1079">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1080" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1080" s="3">
+        <v>44309</v>
+      </c>
+      <c r="B1080" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1080" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1080" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1080" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1080" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1080" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1080" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1080" s="2"/>
+      <c r="J1080" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1080" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1080" s="2">
+        <v>110</v>
+      </c>
+      <c r="M1080" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1080">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1081" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1081" s="3">
+        <v>44309</v>
+      </c>
+      <c r="B1081" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1081" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1081" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1081" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1081" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1081" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1081" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1081" s="2"/>
+      <c r="J1081" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1081" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1081" s="2">
+        <v>-112.4</v>
+      </c>
+      <c r="M1081" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1081">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1082" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1082" s="3">
+        <v>44309</v>
+      </c>
+      <c r="B1082" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C1082" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1082" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1082" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1082" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1082" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1082" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1082" s="2"/>
+      <c r="J1082" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="K1082" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="L1082" s="2">
+        <v>104</v>
+      </c>
+      <c r="M1082" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1082">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1083" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1083" s="3">
+        <v>44309</v>
+      </c>
+      <c r="B1083" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1083" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1083" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1083" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1083" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1083" s="2"/>
+      <c r="H1083" s="2"/>
+      <c r="I1083" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1083" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="K1083" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="L1083" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M1083" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1083">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1084" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1084" s="3">
+        <v>44309</v>
+      </c>
+      <c r="B1084" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1084" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1084" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1084" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1084" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1084" s="2"/>
+      <c r="H1084" s="2"/>
+      <c r="I1084" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1084" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="K1084" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1084" s="2">
+        <v>800</v>
+      </c>
+      <c r="M1084" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1084">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1085" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1085" s="3">
+        <v>44309</v>
+      </c>
+      <c r="B1085" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1085" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1085" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1085" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1085" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1085" s="2"/>
+      <c r="H1085" s="2"/>
+      <c r="I1085" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1085" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="K1085" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="L1085" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M1085" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1085">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1086" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1086" s="3">
+        <v>44309</v>
+      </c>
+      <c r="B1086" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1086" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1086" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1086" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1086" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1086" s="2"/>
+      <c r="H1086" s="2"/>
+      <c r="I1086" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1086" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="K1086" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="L1086" s="2">
+        <v>550</v>
+      </c>
+      <c r="M1086" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1086">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1087" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1087" s="3">
+        <v>44309</v>
+      </c>
+      <c r="B1087" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C1087" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1087" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1087" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1087" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1087" s="2"/>
+      <c r="H1087" s="2"/>
+      <c r="I1087" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1087" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="K1087" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1087" s="2">
+        <v>800</v>
+      </c>
+      <c r="M1087" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1087">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1088" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1088" s="3">
+        <v>44309</v>
+      </c>
+      <c r="B1088" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C1088" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1088" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1088" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1088" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1088" s="2"/>
+      <c r="H1088" s="2"/>
+      <c r="I1088" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1088" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="K1088" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="L1088" s="2">
+        <v>1100</v>
+      </c>
+      <c r="M1088" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1088">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1089" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1089" s="3">
+        <v>44309</v>
+      </c>
+      <c r="B1089" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C1089" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1089" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1089" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1089" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1089" s="2"/>
+      <c r="H1089" s="2"/>
+      <c r="I1089" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1089" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="K1089" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="L1089" s="2">
+        <v>1300</v>
+      </c>
+      <c r="M1089" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1089">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1090" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1090" s="3">
+        <v>44309</v>
+      </c>
+      <c r="B1090" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C1090" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1090" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1090" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1090" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1090" s="2"/>
+      <c r="H1090" s="2"/>
+      <c r="I1090" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1090" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="K1090" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="L1090" s="2">
+        <v>600</v>
+      </c>
+      <c r="M1090" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1090">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1091" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1091" s="3">
+        <v>44309</v>
+      </c>
+      <c r="B1091" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C1091" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1091" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1091" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1091" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1091" s="2"/>
+      <c r="H1091" s="2"/>
+      <c r="I1091" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1091" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="K1091" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="L1091" s="2">
+        <v>900</v>
+      </c>
+      <c r="M1091" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1091">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1092" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1092" s="3">
+        <v>44309</v>
+      </c>
+      <c r="B1092" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1092" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1092" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1092" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1092" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1092" s="2"/>
+      <c r="H1092" s="2"/>
+      <c r="I1092" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1092" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="K1092" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="L1092" s="2">
+        <v>1050</v>
+      </c>
+      <c r="M1092" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1092">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1093" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1093" s="3">
+        <v>44310</v>
+      </c>
+      <c r="B1093" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1093" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1093" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1093" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1093" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1093" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1093" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1093" s="2"/>
+      <c r="J1093" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="K1093" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1093" s="2">
+        <v>120</v>
+      </c>
+      <c r="M1093" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1093">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1094" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1094" s="3">
+        <v>44310</v>
+      </c>
+      <c r="B1094" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1094" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1094" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1094" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1094" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1094" s="2"/>
+      <c r="H1094" s="2"/>
+      <c r="I1094" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1094" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="K1094" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="L1094" s="2">
+        <v>550</v>
+      </c>
+      <c r="M1094" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1094">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1095" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1095" s="3">
+        <v>44310</v>
+      </c>
+      <c r="B1095" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1095" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1095" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1095" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1095" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1095" s="2"/>
+      <c r="H1095" s="2"/>
+      <c r="I1095" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1095" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="K1095" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="L1095" s="2">
+        <v>900</v>
+      </c>
+      <c r="M1095" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1095" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="1096" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1096" s="3">
+        <v>44310</v>
+      </c>
+      <c r="B1096" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1096" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1096" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1096" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1096" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1096" s="2"/>
+      <c r="H1096" s="2"/>
+      <c r="I1096" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1096" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K1096" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="L1096" s="2">
+        <v>500</v>
+      </c>
+      <c r="M1096" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1096">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="1097" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1097" s="3">
+        <v>44310</v>
+      </c>
+      <c r="B1097" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1097" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1097" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1097" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1097" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1097" s="2"/>
+      <c r="H1097" s="2"/>
+      <c r="I1097" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1097" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="K1097" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="L1097" s="2">
+        <v>1200</v>
+      </c>
+      <c r="M1097" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1097">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1098" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1098" s="3">
+        <v>44310</v>
+      </c>
+      <c r="B1098" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1098" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1098" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1098" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1098" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1098" s="2"/>
+      <c r="H1098" s="2"/>
+      <c r="I1098" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1098" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="K1098" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="L1098" s="2">
+        <v>900</v>
+      </c>
+      <c r="M1098" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1098">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="1099" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1099" s="3">
+        <v>44310</v>
+      </c>
+      <c r="B1099" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1099" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1099" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1099" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1099" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1099" s="2"/>
+      <c r="H1099" s="2"/>
+      <c r="I1099" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1099" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K1099" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="L1099" s="2">
+        <v>500</v>
+      </c>
+      <c r="M1099" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1099">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="1100" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1100" s="3">
+        <v>44310</v>
+      </c>
+      <c r="B1100" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C1100" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1100" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1100" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1100" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1100" s="2"/>
+      <c r="H1100" s="2"/>
+      <c r="I1100" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1100" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K1100" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="L1100" s="2">
+        <v>650</v>
+      </c>
+      <c r="M1100" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1101" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1101" s="3">
+        <v>44310</v>
+      </c>
+      <c r="B1101" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C1101" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1101" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1101" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1101" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1101" s="2"/>
+      <c r="H1101" s="2"/>
+      <c r="I1101" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1101" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="K1101" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="L1101" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M1101" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1102" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1102" s="3">
+        <v>44310</v>
+      </c>
+      <c r="B1102" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C1102" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1102" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1102" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1102" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1102" s="2"/>
+      <c r="H1102" s="2"/>
+      <c r="I1102" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1102" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="K1102" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="L1102" s="2">
+        <v>600</v>
+      </c>
+      <c r="M1102" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1103" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1103" s="3">
+        <v>44310</v>
+      </c>
+      <c r="B1103" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1103" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1103" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1103" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1103" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1103" s="2"/>
+      <c r="H1103" s="2"/>
+      <c r="I1103" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1103" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="K1103" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="L1103" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M1103" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1104" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1104" s="3">
+        <v>44311</v>
+      </c>
+      <c r="B1104" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1104" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1104" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1104" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1104" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1104" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1104" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1104" s="2"/>
+      <c r="J1104" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="K1104" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="L1104" s="2">
+        <v>101</v>
+      </c>
+      <c r="M1104" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1104">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1105" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1105" s="3">
+        <v>44311</v>
+      </c>
+      <c r="B1105" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1105" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1105" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1105" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1105" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1105" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1105" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1105" s="2"/>
+      <c r="J1105" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1105" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1105" s="2">
+        <v>-117.6</v>
+      </c>
+      <c r="M1105" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1105">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1106" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1106" s="3">
+        <v>44311</v>
+      </c>
+      <c r="B1106" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1106" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1106" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1106" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1106" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1106" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1106" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1106" s="2"/>
+      <c r="J1106" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="K1106" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1106" s="2">
+        <v>112</v>
+      </c>
+      <c r="M1106" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1106">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1107" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1107" s="3">
+        <v>44311</v>
+      </c>
+      <c r="B1107" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1107" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1107" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1107" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1107" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1107" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1107" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1107" s="2"/>
+      <c r="J1107" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1107" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1107" s="2">
+        <v>100</v>
+      </c>
+      <c r="M1107" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1108" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1108" s="3">
+        <v>44311</v>
+      </c>
+      <c r="B1108" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1108" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="D1108" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1108" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1108" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1108" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1108" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1108" s="2"/>
+      <c r="J1108" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="K1108" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1108" s="2">
+        <v>122</v>
+      </c>
+      <c r="M1108" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1108">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1109" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1109" s="3">
+        <v>44311</v>
+      </c>
+      <c r="B1109" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1109" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1109" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1109" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1109" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1109" s="2"/>
+      <c r="H1109" s="2"/>
+      <c r="I1109" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1109" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="K1109" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="L1109" s="2">
+        <v>750</v>
+      </c>
+      <c r="M1109" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1109">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1110" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1110" s="3">
+        <v>44311</v>
+      </c>
+      <c r="B1110" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1110" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1110" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1110" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1110" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1110" s="2"/>
+      <c r="H1110" s="2"/>
+      <c r="I1110" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1110" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="K1110" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="L1110" s="2">
+        <v>750</v>
+      </c>
+      <c r="M1110" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1110">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="1111" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1111" s="3">
+        <v>44311</v>
+      </c>
+      <c r="B1111" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1111" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="D1111" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1111" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1111" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1111" s="2"/>
+      <c r="H1111" s="2"/>
+      <c r="I1111" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1111" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="K1111" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="L1111" s="2">
+        <v>900</v>
+      </c>
+      <c r="M1111" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1111">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1112" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1112" s="3">
+        <v>44311</v>
+      </c>
+      <c r="B1112" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1112" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1112" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1112" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1112" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1112" s="2"/>
+      <c r="H1112" s="2"/>
+      <c r="I1112" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1112" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="K1112" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="L1112" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M1112" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1113" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1113" s="3">
+        <v>44311</v>
+      </c>
+      <c r="B1113" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1113" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1113" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1113" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1113" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1113" s="2"/>
+      <c r="H1113" s="2"/>
+      <c r="I1113" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1113" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="K1113" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="L1113" s="2">
+        <v>1100</v>
+      </c>
+      <c r="M1113" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1113">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="1114" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1114" s="3">
+        <v>44311</v>
+      </c>
+      <c r="B1114" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1114" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1114" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1114" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1114" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1114" s="2"/>
+      <c r="H1114" s="2"/>
+      <c r="I1114" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1114" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="K1114" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="L1114" s="2">
+        <v>750</v>
+      </c>
+      <c r="M1114" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1114">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="1115" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1115" s="3">
+        <v>44311</v>
+      </c>
+      <c r="B1115" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C1115" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1115" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1115" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1115" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1115" s="2"/>
+      <c r="H1115" s="2"/>
+      <c r="I1115" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1115" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="K1115" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="L1115" s="2">
+        <v>1100</v>
+      </c>
+      <c r="M1115" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1115">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="1116" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1116" s="3">
+        <v>44311</v>
+      </c>
+      <c r="B1116" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C1116" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1116" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1116" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1116" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1116" s="2"/>
+      <c r="H1116" s="2"/>
+      <c r="I1116" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1116" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="K1116" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="L1116" s="2">
+        <v>800</v>
+      </c>
+      <c r="M1116" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1117" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1117" s="3">
+        <v>44311</v>
+      </c>
+      <c r="B1117" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C1117" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1117" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1117" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1117" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1117" s="2"/>
+      <c r="H1117" s="2"/>
+      <c r="I1117" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1117" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="K1117" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="L1117" s="2">
+        <v>850</v>
+      </c>
+      <c r="M1117" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1117">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1118" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1118" s="3">
+        <v>44312</v>
+      </c>
+      <c r="B1118" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1118" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1118" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1118" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1118" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1118" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1118" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1118" s="2"/>
+      <c r="J1118" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="K1118" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="L1118" s="2">
+        <v>-107.5</v>
+      </c>
+      <c r="M1118" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1119" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1119" s="3">
+        <v>44312</v>
+      </c>
+      <c r="B1119" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1119" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1119" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1119" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1119" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1119" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1119" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1119" s="2"/>
+      <c r="J1119" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="K1119" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1119" s="2">
+        <v>116</v>
+      </c>
+      <c r="M1119" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1119">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1120" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1120" s="3">
+        <v>44312</v>
+      </c>
+      <c r="B1120" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1120" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1120" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1120" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1120" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1120" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1120" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1120" s="2"/>
+      <c r="J1120" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1120" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1120" s="2">
+        <v>124</v>
+      </c>
+      <c r="M1120" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1120">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1121" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1121" s="3">
+        <v>44312</v>
+      </c>
+      <c r="B1121" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1121" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1121" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1121" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1121" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1121" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1121" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1121" s="2"/>
+      <c r="J1121" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1121" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1121" s="2">
+        <v>128</v>
+      </c>
+      <c r="M1121" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1122" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1122" s="3">
+        <v>44312</v>
+      </c>
+      <c r="B1122" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1122" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1122" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1122" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1122" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1122" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1122" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1122" s="2"/>
+      <c r="J1122" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1122" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L1122" s="2">
+        <v>114</v>
+      </c>
+      <c r="M1122" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1123" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1123" s="3">
+        <v>44312</v>
+      </c>
+      <c r="B1123" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1123" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1123" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1123" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1123" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1123" s="2"/>
+      <c r="H1123" s="2"/>
+      <c r="I1123" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1123" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K1123" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="L1123" s="2">
+        <v>500</v>
+      </c>
+      <c r="M1123" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1123">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="1124" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1124" s="3">
+        <v>44312</v>
+      </c>
+      <c r="B1124" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1124" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1124" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1124" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1124" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1124" s="2"/>
+      <c r="H1124" s="2"/>
+      <c r="I1124" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1124" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="K1124" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="L1124" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M1124" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1124">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1125" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1125" s="3">
+        <v>44312</v>
+      </c>
+      <c r="B1125" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1125" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1125" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1125" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1125" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1125" s="2"/>
+      <c r="H1125" s="2"/>
+      <c r="I1125" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1125" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="K1125" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="L1125" s="2">
+        <v>600</v>
+      </c>
+      <c r="M1125" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1125">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1126" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1126" s="3">
+        <v>44312</v>
+      </c>
+      <c r="B1126" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1126" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1126" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1126" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1126" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1126" s="2"/>
+      <c r="H1126" s="2"/>
+      <c r="I1126" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1126" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="K1126" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="L1126" s="2">
+        <v>950</v>
+      </c>
+      <c r="M1126" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1126">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1127" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1127" s="3">
+        <v>44312</v>
+      </c>
+      <c r="B1127" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1127" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1127" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1127" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1127" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1127" s="2"/>
+      <c r="H1127" s="2"/>
+      <c r="I1127" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1127" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K1127" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="L1127" s="2">
+        <v>500</v>
+      </c>
+      <c r="M1127" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1127">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="1128" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1128" s="3">
+        <v>44312</v>
+      </c>
+      <c r="B1128" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1128" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1128" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1128" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1128" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1128" s="2"/>
+      <c r="H1128" s="2"/>
+      <c r="I1128" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1128" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="K1128" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="L1128" s="2">
+        <v>800</v>
+      </c>
+      <c r="M1128" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1128">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1129" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1129" s="3">
+        <v>44312</v>
+      </c>
+      <c r="B1129" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1129" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1129" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1129" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1129" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1129" s="2"/>
+      <c r="H1129" s="2"/>
+      <c r="I1129" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1129" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="K1129" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="L1129" s="2">
+        <v>900</v>
+      </c>
+      <c r="M1129" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1130" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1130" s="3">
+        <v>44312</v>
+      </c>
+      <c r="B1130" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1130" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1130" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1130" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1130" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1130" s="2"/>
+      <c r="H1130" s="2"/>
+      <c r="I1130" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1130" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="K1130" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="L1130" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M1130" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1130">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="1131" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1131" s="3">
+        <v>44312</v>
+      </c>
+      <c r="B1131" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C1131" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1131" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1131" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1131" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1131" s="2"/>
+      <c r="H1131" s="2"/>
+      <c r="I1131" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1131" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="K1131" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="L1131" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M1131" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1131">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="1132" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1132" s="3">
+        <v>44312</v>
+      </c>
+      <c r="B1132" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C1132" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1132" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1132" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1132" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1132" s="2"/>
+      <c r="H1132" s="2"/>
+      <c r="I1132" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1132" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="K1132" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="L1132" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M1132" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1132">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1133" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1133" s="3">
+        <v>44312</v>
+      </c>
+      <c r="B1133" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C1133" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1133" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1133" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1133" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1133" s="2"/>
+      <c r="H1133" s="2"/>
+      <c r="I1133" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1133" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="K1133" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="L1133" s="2">
+        <v>800</v>
+      </c>
+      <c r="M1133" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1133">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1134" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1134" s="3">
+        <v>44312</v>
+      </c>
+      <c r="B1134" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1134" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1134" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1134" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1134" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1134" s="2"/>
+      <c r="H1134" s="2"/>
+      <c r="I1134" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1134" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="K1134" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="L1134" s="2">
+        <v>900</v>
+      </c>
+      <c r="M1134" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1134">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="1135" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1135" s="3">
+        <v>44312</v>
+      </c>
+      <c r="B1135" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1135" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1135" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1135" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1135" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1135" s="2"/>
+      <c r="H1135" s="2"/>
+      <c r="I1135" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1135" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="K1135" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="L1135" s="2">
+        <v>550</v>
+      </c>
+      <c r="M1135" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1135">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="1136" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1136" s="3">
+        <v>44312</v>
+      </c>
+      <c r="B1136" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C1136" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1136" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1136" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1136" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1136" s="2"/>
+      <c r="H1136" s="2"/>
+      <c r="I1136" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1136" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="K1136" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="L1136" s="2">
+        <v>550</v>
+      </c>
+      <c r="M1136" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1136">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="1137" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1137" s="3">
+        <v>44312</v>
+      </c>
+      <c r="B1137" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C1137" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1137" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1137" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1137" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1137" s="2"/>
+      <c r="H1137" s="2"/>
+      <c r="I1137" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1137" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="K1137" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="L1137" s="2">
+        <v>750</v>
+      </c>
+      <c r="M1137" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1137">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1138" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1138" s="3">
+        <v>44312</v>
+      </c>
+      <c r="B1138" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C1138" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1138" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1138" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1138" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1138" s="2"/>
+      <c r="H1138" s="2"/>
+      <c r="I1138" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1138" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="K1138" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="L1138" s="2">
+        <v>900</v>
+      </c>
+      <c r="M1138" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1138">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="1139" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1139" s="3">
+        <v>44312</v>
+      </c>
+      <c r="B1139" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1139" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1139" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1139" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1139" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1139" s="2"/>
+      <c r="H1139" s="2"/>
+      <c r="I1139" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1139" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="K1139" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="L1139" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M1139" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1139">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="1140" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1140" s="3">
+        <v>44312</v>
+      </c>
+      <c r="B1140" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C1140" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1140" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1140" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1140" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1140" s="2"/>
+      <c r="H1140" s="2"/>
+      <c r="I1140" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1140" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="K1140" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="L1140" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M1140" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1140" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="1141" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1141" s="3">
+        <v>44312</v>
+      </c>
+      <c r="B1141" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1141" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1141" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1141" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1141" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1141" s="2"/>
+      <c r="H1141" s="2"/>
+      <c r="I1141" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1141" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="K1141" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="L1141" s="2">
+        <v>950</v>
+      </c>
+      <c r="M1141" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1141">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1142" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1142" s="3">
+        <v>44312</v>
+      </c>
+      <c r="B1142" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1142" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1142" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E1142" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1142" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1142" s="2"/>
+      <c r="H1142" s="2"/>
+      <c r="I1142" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1142" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="K1142" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="L1142" s="2">
+        <v>950</v>
+      </c>
+      <c r="M1142" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1142">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A634:M642 A874:H878 J874:J878 A916:M948 A965:M999 A1011:K1023 L1011:M1022 A1024:M1036">
-    <cfRule type="expression" dxfId="45" priority="38">
+  <conditionalFormatting sqref="A634:M642 A874:H878 J874:J878 A916:M948 A965:M999 A1011:K1023 L1011:M1022 A1024:M1036 A1079:M1103 N1095 A1118:M1142 N1140">
+    <cfRule type="expression" dxfId="46" priority="42">
       <formula>$B634=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A503:B521">
-    <cfRule type="expression" dxfId="44" priority="55">
+    <cfRule type="expression" dxfId="45" priority="59">
       <formula>$B503=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C503:D521">
-    <cfRule type="expression" dxfId="43" priority="54">
+    <cfRule type="expression" dxfId="44" priority="58">
       <formula>$B503=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E503:I521">
-    <cfRule type="expression" dxfId="42" priority="53">
+    <cfRule type="expression" dxfId="43" priority="57">
       <formula>$B503=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J503:J521">
-    <cfRule type="expression" dxfId="41" priority="52">
+    <cfRule type="expression" dxfId="42" priority="56">
       <formula>$B503=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K503:K521">
-    <cfRule type="expression" dxfId="40" priority="51">
+    <cfRule type="expression" dxfId="41" priority="55">
       <formula>$B503=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L503:M521">
-    <cfRule type="expression" dxfId="39" priority="50">
+    <cfRule type="expression" dxfId="40" priority="54">
       <formula>$B503=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A522:B551">
-    <cfRule type="expression" dxfId="38" priority="49">
+    <cfRule type="expression" dxfId="39" priority="53">
       <formula>$B522=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C522:D551">
-    <cfRule type="expression" dxfId="37" priority="48">
+    <cfRule type="expression" dxfId="38" priority="52">
       <formula>$B522=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E522:I551">
-    <cfRule type="expression" dxfId="36" priority="47">
+    <cfRule type="expression" dxfId="37" priority="51">
       <formula>$B522=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J522:J551">
-    <cfRule type="expression" dxfId="35" priority="46">
+    <cfRule type="expression" dxfId="36" priority="50">
       <formula>$B522=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K522:K551">
-    <cfRule type="expression" dxfId="34" priority="45">
+    <cfRule type="expression" dxfId="35" priority="49">
       <formula>$B522=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L522:M551">
-    <cfRule type="expression" dxfId="33" priority="44">
+    <cfRule type="expression" dxfId="34" priority="48">
       <formula>$B522=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A552:M561">
-    <cfRule type="expression" dxfId="32" priority="43">
+    <cfRule type="expression" dxfId="33" priority="47">
       <formula>$B552=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A562:M588">
-    <cfRule type="expression" dxfId="31" priority="42">
+    <cfRule type="expression" dxfId="32" priority="46">
       <formula>$B562=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A589:M599">
-    <cfRule type="expression" dxfId="30" priority="41">
+    <cfRule type="expression" dxfId="31" priority="45">
       <formula>$B589=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A600:M611">
-    <cfRule type="expression" dxfId="29" priority="40">
+    <cfRule type="expression" dxfId="30" priority="44">
       <formula>$B600=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A612:M633">
-    <cfRule type="expression" dxfId="28" priority="39">
+    <cfRule type="expression" dxfId="29" priority="43">
       <formula>$B612=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A643:M665">
-    <cfRule type="expression" dxfId="27" priority="37">
+    <cfRule type="expression" dxfId="28" priority="41">
       <formula>$B643=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A666:B675">
-    <cfRule type="expression" dxfId="26" priority="36">
+    <cfRule type="expression" dxfId="27" priority="40">
       <formula>$B666=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C666:D675">
-    <cfRule type="expression" dxfId="25" priority="35">
+    <cfRule type="expression" dxfId="26" priority="39">
       <formula>$B666=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E666:J675">
-    <cfRule type="expression" dxfId="24" priority="34">
+    <cfRule type="expression" dxfId="25" priority="38">
       <formula>$B666=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K666:K675">
-    <cfRule type="expression" dxfId="23" priority="33">
+    <cfRule type="expression" dxfId="24" priority="37">
       <formula>$B666=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L666:M675">
-    <cfRule type="expression" dxfId="22" priority="32">
+    <cfRule type="expression" dxfId="23" priority="36">
       <formula>$B666=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A676:B698">
-    <cfRule type="expression" dxfId="21" priority="31">
+    <cfRule type="expression" dxfId="22" priority="35">
       <formula>$B676=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C676:D698">
-    <cfRule type="expression" dxfId="20" priority="30">
+    <cfRule type="expression" dxfId="21" priority="34">
       <formula>$B676=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E676:J698">
-    <cfRule type="expression" dxfId="19" priority="29">
+    <cfRule type="expression" dxfId="20" priority="33">
       <formula>$B676=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K676:K698">
-    <cfRule type="expression" dxfId="18" priority="28">
+    <cfRule type="expression" dxfId="19" priority="32">
       <formula>$B676=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L676:M698">
-    <cfRule type="expression" dxfId="17" priority="27">
+    <cfRule type="expression" dxfId="18" priority="31">
       <formula>$B676=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A699:M713">
-    <cfRule type="expression" dxfId="16" priority="26">
+    <cfRule type="expression" dxfId="17" priority="30">
       <formula>$B699=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A714:M729">
-    <cfRule type="expression" dxfId="15" priority="25">
+    <cfRule type="expression" dxfId="16" priority="29">
       <formula>$B714=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A730:M747">
-    <cfRule type="expression" dxfId="14" priority="24">
+    <cfRule type="expression" dxfId="15" priority="28">
       <formula>$B730=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A748:M768">
-    <cfRule type="expression" dxfId="13" priority="23">
+    <cfRule type="expression" dxfId="14" priority="27">
       <formula>$B748=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A769:M791">
-    <cfRule type="expression" dxfId="12" priority="22">
+    <cfRule type="expression" dxfId="13" priority="26">
       <formula>$B769=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A792:M812">
-    <cfRule type="expression" dxfId="11" priority="21">
+    <cfRule type="expression" dxfId="12" priority="25">
       <formula>$B792=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A813:M835">
-    <cfRule type="expression" dxfId="10" priority="20">
+    <cfRule type="expression" dxfId="11" priority="24">
       <formula>$B813=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A836:M847">
-    <cfRule type="expression" dxfId="9" priority="19">
+    <cfRule type="expression" dxfId="10" priority="23">
       <formula>$B836=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A848:M873">
-    <cfRule type="expression" dxfId="8" priority="18">
+    <cfRule type="expression" dxfId="9" priority="22">
       <formula>$B848=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K874:M878">
-    <cfRule type="expression" dxfId="7" priority="14">
+    <cfRule type="expression" dxfId="8" priority="18">
       <formula>$B874=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A879:M898">
-    <cfRule type="expression" dxfId="6" priority="15">
+    <cfRule type="expression" dxfId="7" priority="19">
       <formula>$B879=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A899:M915">
-    <cfRule type="expression" dxfId="5" priority="13">
+    <cfRule type="expression" dxfId="6" priority="17">
       <formula>$B899=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A949:M964">
-    <cfRule type="expression" dxfId="4" priority="11">
+    <cfRule type="expression" dxfId="5" priority="15">
       <formula>$B949=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1000:M1010">
-    <cfRule type="expression" dxfId="3" priority="7">
+    <cfRule type="expression" dxfId="4" priority="11">
       <formula>$B1000=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1023:M1023">
-    <cfRule type="expression" dxfId="2" priority="4">
+    <cfRule type="expression" dxfId="3" priority="8">
       <formula>$B1023=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1037:M1061">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="2" priority="6">
       <formula>$B1037=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1062:M1078">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="1" priority="5">
       <formula>$B1062=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1104:M1117">
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>$B1104=""</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
prop bet tracker updates
</commit_message>
<xml_diff>
--- a/scratch/Prop Bets.xlsx
+++ b/scratch/Prop Bets.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kjzk13/Desktop/Fun/Betting/Models/Git/NBA/data_repos/gambling_stuff/scratch/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93BB922B-8629-044D-97BC-C3273E68840E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63B50B54-1DB1-B641-B0F3-425C6349BED6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16220" xr2:uid="{A921039E-F491-3040-A02B-E90974210F5A}"/>
+    <workbookView xWindow="28800" yWindow="-1120" windowWidth="38400" windowHeight="21600" xr2:uid="{A921039E-F491-3040-A02B-E90974210F5A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="13" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$N$1176</definedName>
     <definedName name="Pending">#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10549" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10862" uniqueCount="278">
   <si>
     <t>Date</t>
   </si>
@@ -865,6 +866,12 @@
   <si>
     <t>Furkan Korkmaz</t>
   </si>
+  <si>
+    <t>Chimezie Metu</t>
+  </si>
+  <si>
+    <t>Tremont Waters</t>
+  </si>
 </sst>
 </file>
 
@@ -924,7 +931,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="47">
+  <dxfs count="49">
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color theme="0" tint="-0.499984740745262"/>
@@ -1470,10 +1487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C79C926B-E4E0-6445-8BE2-2104EE8EA8CE}">
-  <dimension ref="A1:N1142"/>
+  <dimension ref="A1:N1176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1112" workbookViewId="0">
-      <selection activeCell="N1143" sqref="N1143"/>
+    <sheetView tabSelected="1" topLeftCell="A1144" workbookViewId="0">
+      <selection activeCell="D1176" sqref="D1176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -46266,7 +46283,7 @@
         <v>5</v>
       </c>
       <c r="F1107" s="2" t="s">
-        <v>137</v>
+        <v>62</v>
       </c>
       <c r="G1107" s="2" t="s">
         <v>9</v>
@@ -46308,7 +46325,7 @@
         <v>5</v>
       </c>
       <c r="F1108" s="2" t="s">
-        <v>137</v>
+        <v>62</v>
       </c>
       <c r="G1108" s="2" t="s">
         <v>9</v>
@@ -47703,240 +47720,1625 @@
         <v>1</v>
       </c>
     </row>
+    <row r="1143" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1143" s="3">
+        <v>44313</v>
+      </c>
+      <c r="B1143" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1143" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1143" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1143" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1143" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1143" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1143" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1143" s="2"/>
+      <c r="J1143" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1143" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1143" s="2">
+        <v>108</v>
+      </c>
+      <c r="M1143" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1143">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1144" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1144" s="3">
+        <v>44313</v>
+      </c>
+      <c r="B1144" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1144" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1144" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1144" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1144" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1144" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1144" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1144" s="2"/>
+      <c r="J1144" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1144" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1144" s="2">
+        <v>122</v>
+      </c>
+      <c r="M1144" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1144">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1145" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1145" s="3">
+        <v>44313</v>
+      </c>
+      <c r="B1145" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1145" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1145" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1145" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1145" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1145" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1145" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1145" s="2"/>
+      <c r="J1145" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K1145" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1145" s="2">
+        <v>-112.4</v>
+      </c>
+      <c r="M1145" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1145">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1146" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1146" s="3">
+        <v>44313</v>
+      </c>
+      <c r="B1146" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1146" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1146" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1146" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1146" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1146" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1146" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1146" s="2"/>
+      <c r="J1146" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="K1146" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="L1146" s="2">
+        <v>138</v>
+      </c>
+      <c r="M1146" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1146">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1147" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1147" s="3">
+        <v>44313</v>
+      </c>
+      <c r="B1147" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1147" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1147" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1147" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1147" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1147" s="2"/>
+      <c r="H1147" s="2"/>
+      <c r="I1147" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1147" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="K1147" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="L1147" s="2">
+        <v>900</v>
+      </c>
+      <c r="M1147" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1147">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="1148" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1148" s="3">
+        <v>44313</v>
+      </c>
+      <c r="B1148" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1148" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1148" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1148" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1148" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1148" s="2"/>
+      <c r="H1148" s="2"/>
+      <c r="I1148" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1148" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="K1148" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="L1148" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M1148" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1148">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1149" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1149" s="3">
+        <v>44313</v>
+      </c>
+      <c r="B1149" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C1149" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1149" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1149" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1149" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1149" s="2"/>
+      <c r="H1149" s="2"/>
+      <c r="I1149" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1149" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="K1149" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="L1149" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M1149" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1149">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1150" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1150" s="3">
+        <v>44313</v>
+      </c>
+      <c r="B1150" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C1150" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1150" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1150" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1150" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1150" s="2"/>
+      <c r="H1150" s="2"/>
+      <c r="I1150" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1150" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="K1150" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="L1150" s="2">
+        <v>600</v>
+      </c>
+      <c r="M1150" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1150">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1151" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1151" s="3">
+        <v>44313</v>
+      </c>
+      <c r="B1151" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C1151" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1151" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1151" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1151" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1151" s="2"/>
+      <c r="H1151" s="2"/>
+      <c r="I1151" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1151" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="K1151" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="L1151" s="2">
+        <v>900</v>
+      </c>
+      <c r="M1151" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1151">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="1152" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1152" s="3">
+        <v>44313</v>
+      </c>
+      <c r="B1152" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C1152" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1152" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1152" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1152" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1152" s="2"/>
+      <c r="H1152" s="2"/>
+      <c r="I1152" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1152" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="K1152" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="L1152" s="2">
+        <v>900</v>
+      </c>
+      <c r="M1152" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1152">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1153" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1153" s="3">
+        <v>44313</v>
+      </c>
+      <c r="B1153" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1153" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1153" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1153" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1153" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1153" s="2"/>
+      <c r="H1153" s="2"/>
+      <c r="I1153" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1153" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K1153" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="L1153" s="2">
+        <v>460</v>
+      </c>
+      <c r="M1153" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1153">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1154" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1154" s="3">
+        <v>44314</v>
+      </c>
+      <c r="B1154" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1154" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1154" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1154" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1154" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1154" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1154" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1154" s="2"/>
+      <c r="J1154" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1154" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1154" s="2">
+        <v>-106.4</v>
+      </c>
+      <c r="M1154" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1154">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1155" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1155" s="3">
+        <v>44314</v>
+      </c>
+      <c r="B1155" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1155" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1155" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1155" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1155" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1155" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1155" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1155" s="2"/>
+      <c r="J1155" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="K1155" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1155" s="2">
+        <v>120</v>
+      </c>
+      <c r="M1155" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1155">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1156" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1156" s="3">
+        <v>44314</v>
+      </c>
+      <c r="B1156" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C1156" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1156" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1156" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1156" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1156" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1156" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1156" s="2"/>
+      <c r="J1156" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1156" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1156" s="2">
+        <v>-109.9</v>
+      </c>
+      <c r="M1156" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1156">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1157" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1157" s="3">
+        <v>44314</v>
+      </c>
+      <c r="B1157" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1157" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1157" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1157" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1157" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1157" s="2"/>
+      <c r="H1157" s="2"/>
+      <c r="I1157" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1157" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="K1157" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="L1157" s="2">
+        <v>900</v>
+      </c>
+      <c r="M1157" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1157">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1158" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1158" s="3">
+        <v>44314</v>
+      </c>
+      <c r="B1158" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1158" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1158" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1158" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1158" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1158" s="2"/>
+      <c r="H1158" s="2"/>
+      <c r="I1158" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1158" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="K1158" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="L1158" s="2">
+        <v>550</v>
+      </c>
+      <c r="M1158" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1159" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1159" s="3">
+        <v>44314</v>
+      </c>
+      <c r="B1159" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1159" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1159" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1159" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1159" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1159" s="2"/>
+      <c r="H1159" s="2"/>
+      <c r="I1159" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1159" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="K1159" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="L1159" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M1159" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1159">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="1160" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1160" s="3">
+        <v>44314</v>
+      </c>
+      <c r="B1160" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1160" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1160" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1160" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1160" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1160" s="2"/>
+      <c r="H1160" s="2"/>
+      <c r="I1160" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1160" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="K1160" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="L1160" s="2">
+        <v>900</v>
+      </c>
+      <c r="M1160" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1160">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1161" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1161" s="3">
+        <v>44314</v>
+      </c>
+      <c r="B1161" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1161" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1161" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1161" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1161" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1161" s="2"/>
+      <c r="H1161" s="2"/>
+      <c r="I1161" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1161" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="K1161" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="L1161" s="2">
+        <v>500</v>
+      </c>
+      <c r="M1161" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1161">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1162" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1162" s="3">
+        <v>44314</v>
+      </c>
+      <c r="B1162" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1162" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1162" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1162" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1162" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1162" s="2"/>
+      <c r="H1162" s="2"/>
+      <c r="I1162" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1162" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="K1162" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="L1162" s="2">
+        <v>600</v>
+      </c>
+      <c r="M1162" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1162">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1163" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1163" s="3">
+        <v>44314</v>
+      </c>
+      <c r="B1163" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1163" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1163" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1163" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1163" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1163" s="2"/>
+      <c r="H1163" s="2"/>
+      <c r="I1163" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1163" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="K1163" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1163" s="2">
+        <v>900</v>
+      </c>
+      <c r="M1163" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1163">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="1164" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1164" s="3">
+        <v>44314</v>
+      </c>
+      <c r="B1164" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1164" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1164" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1164" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1164" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1164" s="2"/>
+      <c r="H1164" s="2"/>
+      <c r="I1164" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1164" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="K1164" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="L1164" s="2">
+        <v>900</v>
+      </c>
+      <c r="M1164" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1164">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="1165" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1165" s="3">
+        <v>44314</v>
+      </c>
+      <c r="B1165" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1165" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1165" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1165" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1165" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1165" s="2"/>
+      <c r="H1165" s="2"/>
+      <c r="I1165" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1165" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="K1165" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="L1165" s="2">
+        <v>1200</v>
+      </c>
+      <c r="M1165" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1165">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1166" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1166" s="3">
+        <v>44314</v>
+      </c>
+      <c r="B1166" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1166" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1166" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1166" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1166" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1166" s="2"/>
+      <c r="H1166" s="2"/>
+      <c r="I1166" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1166" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="K1166" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="L1166" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M1166" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1166">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="1167" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1167" s="3">
+        <v>44314</v>
+      </c>
+      <c r="B1167" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1167" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1167" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1167" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1167" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1167" s="2"/>
+      <c r="H1167" s="2"/>
+      <c r="I1167" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1167" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="K1167" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="L1167" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M1167" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1167">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="1168" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1168" s="3">
+        <v>44314</v>
+      </c>
+      <c r="B1168" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1168" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1168" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1168" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1168" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1168" s="2"/>
+      <c r="H1168" s="2"/>
+      <c r="I1168" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1168" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="K1168" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="L1168" s="2">
+        <v>750</v>
+      </c>
+      <c r="M1168" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1168">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="1169" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1169" s="3">
+        <v>44314</v>
+      </c>
+      <c r="B1169" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C1169" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1169" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1169" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1169" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1169" s="2"/>
+      <c r="H1169" s="2"/>
+      <c r="I1169" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1169" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="K1169" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="L1169" s="2">
+        <v>900</v>
+      </c>
+      <c r="M1169" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1169">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="1170" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1170" s="3">
+        <v>44314</v>
+      </c>
+      <c r="B1170" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C1170" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1170" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1170" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1170" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1170" s="2"/>
+      <c r="H1170" s="2"/>
+      <c r="I1170" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1170" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="K1170" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1170" s="2">
+        <v>900</v>
+      </c>
+      <c r="M1170" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1170">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="1171" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1171" s="3">
+        <v>44314</v>
+      </c>
+      <c r="B1171" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C1171" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1171" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1171" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1171" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1171" s="2"/>
+      <c r="H1171" s="2"/>
+      <c r="I1171" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1171" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="K1171" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="L1171" s="2">
+        <v>800</v>
+      </c>
+      <c r="M1171" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1171">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1172" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1172" s="3">
+        <v>44314</v>
+      </c>
+      <c r="B1172" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C1172" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1172" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1172" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1172" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1172" s="2"/>
+      <c r="H1172" s="2"/>
+      <c r="I1172" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1172" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="K1172" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="L1172" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M1172" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1172">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="1173" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1173" s="3">
+        <v>44314</v>
+      </c>
+      <c r="B1173" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C1173" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1173" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1173" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1173" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1173" s="2"/>
+      <c r="H1173" s="2"/>
+      <c r="I1173" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1173" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="K1173" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="L1173" s="2">
+        <v>750</v>
+      </c>
+      <c r="M1173" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1173">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="1174" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1174" s="3">
+        <v>44314</v>
+      </c>
+      <c r="B1174" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1174" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1174" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1174" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1174" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1174" s="2"/>
+      <c r="H1174" s="2"/>
+      <c r="I1174" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1174" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="K1174" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="L1174" s="2">
+        <v>900</v>
+      </c>
+      <c r="M1174" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1174">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="1175" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1175" s="3">
+        <v>44314</v>
+      </c>
+      <c r="B1175" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C1175" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1175" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1175" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1175" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1175" s="2"/>
+      <c r="H1175" s="2"/>
+      <c r="I1175" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1175" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="K1175" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="L1175" s="2">
+        <v>900</v>
+      </c>
+      <c r="M1175" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1175">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="1176" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1176" s="3">
+        <v>44314</v>
+      </c>
+      <c r="B1176" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1176" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1176" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1176" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1176" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1176" s="2"/>
+      <c r="H1176" s="2"/>
+      <c r="I1176" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1176" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="K1176" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="L1176" s="2">
+        <v>700</v>
+      </c>
+      <c r="M1176" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1176">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:N1176" xr:uid="{D9DA4A53-0950-BF46-87A1-1C9C0384F4A7}"/>
   <conditionalFormatting sqref="A634:M642 A874:H878 J874:J878 A916:M948 A965:M999 A1011:K1023 L1011:M1022 A1024:M1036 A1079:M1103 N1095 A1118:M1142 N1140">
-    <cfRule type="expression" dxfId="46" priority="42">
+    <cfRule type="expression" dxfId="48" priority="44">
       <formula>$B634=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A503:B521">
+    <cfRule type="expression" dxfId="47" priority="61">
+      <formula>$B503=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C503:D521">
+    <cfRule type="expression" dxfId="46" priority="60">
+      <formula>$B503=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E503:I521">
     <cfRule type="expression" dxfId="45" priority="59">
       <formula>$B503=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C503:D521">
+  <conditionalFormatting sqref="J503:J521">
     <cfRule type="expression" dxfId="44" priority="58">
       <formula>$B503=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E503:I521">
+  <conditionalFormatting sqref="K503:K521">
     <cfRule type="expression" dxfId="43" priority="57">
       <formula>$B503=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J503:J521">
+  <conditionalFormatting sqref="L503:M521">
     <cfRule type="expression" dxfId="42" priority="56">
       <formula>$B503=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K503:K521">
+  <conditionalFormatting sqref="A522:B551">
     <cfRule type="expression" dxfId="41" priority="55">
-      <formula>$B503=""</formula>
+      <formula>$B522=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L503:M521">
+  <conditionalFormatting sqref="C522:D551">
     <cfRule type="expression" dxfId="40" priority="54">
-      <formula>$B503=""</formula>
+      <formula>$B522=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A522:B551">
+  <conditionalFormatting sqref="E522:I551">
     <cfRule type="expression" dxfId="39" priority="53">
       <formula>$B522=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C522:D551">
+  <conditionalFormatting sqref="J522:J551">
     <cfRule type="expression" dxfId="38" priority="52">
       <formula>$B522=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E522:I551">
+  <conditionalFormatting sqref="K522:K551">
     <cfRule type="expression" dxfId="37" priority="51">
       <formula>$B522=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J522:J551">
+  <conditionalFormatting sqref="L522:M551">
     <cfRule type="expression" dxfId="36" priority="50">
       <formula>$B522=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K522:K551">
+  <conditionalFormatting sqref="A552:M561">
     <cfRule type="expression" dxfId="35" priority="49">
-      <formula>$B522=""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L522:M551">
-    <cfRule type="expression" dxfId="34" priority="48">
-      <formula>$B522=""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A552:M561">
-    <cfRule type="expression" dxfId="33" priority="47">
       <formula>$B552=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A562:M588">
-    <cfRule type="expression" dxfId="32" priority="46">
+    <cfRule type="expression" dxfId="34" priority="48">
       <formula>$B562=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A589:M599">
-    <cfRule type="expression" dxfId="31" priority="45">
+    <cfRule type="expression" dxfId="33" priority="47">
       <formula>$B589=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A600:M611">
-    <cfRule type="expression" dxfId="30" priority="44">
+    <cfRule type="expression" dxfId="32" priority="46">
       <formula>$B600=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A612:M633">
-    <cfRule type="expression" dxfId="29" priority="43">
+    <cfRule type="expression" dxfId="31" priority="45">
       <formula>$B612=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A643:M665">
-    <cfRule type="expression" dxfId="28" priority="41">
+    <cfRule type="expression" dxfId="30" priority="43">
       <formula>$B643=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A666:B675">
+    <cfRule type="expression" dxfId="29" priority="42">
+      <formula>$B666=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C666:D675">
+    <cfRule type="expression" dxfId="28" priority="41">
+      <formula>$B666=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E666:J675">
     <cfRule type="expression" dxfId="27" priority="40">
       <formula>$B666=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C666:D675">
+  <conditionalFormatting sqref="K666:K675">
     <cfRule type="expression" dxfId="26" priority="39">
       <formula>$B666=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E666:J675">
+  <conditionalFormatting sqref="L666:M675">
     <cfRule type="expression" dxfId="25" priority="38">
       <formula>$B666=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K666:K675">
+  <conditionalFormatting sqref="A676:B698">
     <cfRule type="expression" dxfId="24" priority="37">
-      <formula>$B666=""</formula>
+      <formula>$B676=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L666:M675">
+  <conditionalFormatting sqref="C676:D698">
     <cfRule type="expression" dxfId="23" priority="36">
-      <formula>$B666=""</formula>
+      <formula>$B676=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A676:B698">
+  <conditionalFormatting sqref="E676:J698">
     <cfRule type="expression" dxfId="22" priority="35">
       <formula>$B676=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C676:D698">
+  <conditionalFormatting sqref="K676:K698">
     <cfRule type="expression" dxfId="21" priority="34">
       <formula>$B676=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E676:J698">
+  <conditionalFormatting sqref="L676:M698">
     <cfRule type="expression" dxfId="20" priority="33">
       <formula>$B676=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K676:K698">
+  <conditionalFormatting sqref="A699:M713">
     <cfRule type="expression" dxfId="19" priority="32">
-      <formula>$B676=""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L676:M698">
-    <cfRule type="expression" dxfId="18" priority="31">
-      <formula>$B676=""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A699:M713">
-    <cfRule type="expression" dxfId="17" priority="30">
       <formula>$B699=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A714:M729">
-    <cfRule type="expression" dxfId="16" priority="29">
+    <cfRule type="expression" dxfId="18" priority="31">
       <formula>$B714=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A730:M747">
-    <cfRule type="expression" dxfId="15" priority="28">
+    <cfRule type="expression" dxfId="17" priority="30">
       <formula>$B730=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A748:M768">
-    <cfRule type="expression" dxfId="14" priority="27">
+    <cfRule type="expression" dxfId="16" priority="29">
       <formula>$B748=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A769:M791">
-    <cfRule type="expression" dxfId="13" priority="26">
+    <cfRule type="expression" dxfId="15" priority="28">
       <formula>$B769=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A792:M812">
-    <cfRule type="expression" dxfId="12" priority="25">
+    <cfRule type="expression" dxfId="14" priority="27">
       <formula>$B792=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A813:M835">
-    <cfRule type="expression" dxfId="11" priority="24">
+    <cfRule type="expression" dxfId="13" priority="26">
       <formula>$B813=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A836:M847">
-    <cfRule type="expression" dxfId="10" priority="23">
+    <cfRule type="expression" dxfId="12" priority="25">
       <formula>$B836=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A848:M873">
-    <cfRule type="expression" dxfId="9" priority="22">
+    <cfRule type="expression" dxfId="11" priority="24">
       <formula>$B848=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K874:M878">
-    <cfRule type="expression" dxfId="8" priority="18">
+    <cfRule type="expression" dxfId="10" priority="20">
       <formula>$B874=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A879:M898">
-    <cfRule type="expression" dxfId="7" priority="19">
+    <cfRule type="expression" dxfId="9" priority="21">
       <formula>$B879=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A899:M915">
-    <cfRule type="expression" dxfId="6" priority="17">
+    <cfRule type="expression" dxfId="8" priority="19">
       <formula>$B899=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A949:M964">
-    <cfRule type="expression" dxfId="5" priority="15">
+    <cfRule type="expression" dxfId="7" priority="17">
       <formula>$B949=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1000:M1010">
-    <cfRule type="expression" dxfId="4" priority="11">
+    <cfRule type="expression" dxfId="6" priority="13">
       <formula>$B1000=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1023:M1023">
-    <cfRule type="expression" dxfId="3" priority="8">
+    <cfRule type="expression" dxfId="5" priority="10">
       <formula>$B1023=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1037:M1061">
-    <cfRule type="expression" dxfId="2" priority="6">
+    <cfRule type="expression" dxfId="4" priority="8">
       <formula>$B1037=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1062:M1078">
-    <cfRule type="expression" dxfId="1" priority="5">
+    <cfRule type="expression" dxfId="3" priority="7">
       <formula>$B1062=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1104:M1117">
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="2" priority="4">
       <formula>$B1104=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1143:M1153">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>$B1143=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1154:M1176">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$B1154=""</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>